<commit_message>
Obtained up/down differential asymmetry. Potentially obtained correct shape for A_EDM vs p, by dividing by maximum angular difference per momentum bin. More work needed.
</commit_message>
<xml_diff>
--- a/Sheets/RadialFieldErrors.xlsx
+++ b/Sheets/RadialFieldErrors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E03BAE6-32D3-A54E-B8A1-93E24E530DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FC39DA-CA28-A545-9C2B-C8B24FA367E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15240" yWindow="720" windowWidth="13560" windowHeight="16940" xr2:uid="{1195E68F-FC63-AD4A-8502-4C781A649C79}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>